<commit_message>
Add score rule "No 2 shifts within 10 hours from each other" + fix generator
</commit_message>
<xml_diff>
--- a/optaplanner-training-lab902-solution/data/workerrostering/import/roster-10spots-7days.xlsx
+++ b/optaplanner-training-lab902-solution/data/workerrostering/import/roster-10spots-7days.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="90">
   <si>
     <t>Name</t>
   </si>
@@ -119,6 +119,78 @@
   </si>
   <si>
     <t>Amy A. P. Fox</t>
+  </si>
+  <si>
+    <t>Beth B. Q. Green</t>
+  </si>
+  <si>
+    <t>Chad C. R. Jones</t>
+  </si>
+  <si>
+    <t>Dan D. S. King</t>
+  </si>
+  <si>
+    <t>Elsa E. T. Li</t>
+  </si>
+  <si>
+    <t>Flo F. U. Poe</t>
+  </si>
+  <si>
+    <t>Gus G. V. Rye</t>
+  </si>
+  <si>
+    <t>Hugo H. W. Smith</t>
+  </si>
+  <si>
+    <t>Ivy I. X. Watt</t>
+  </si>
+  <si>
+    <t>Jay J. O. Cole</t>
+  </si>
+  <si>
+    <t>Amy A. Q. Green</t>
+  </si>
+  <si>
+    <t>Beth B. R. Jones</t>
+  </si>
+  <si>
+    <t>Chad C. S. King</t>
+  </si>
+  <si>
+    <t>Dan D. T. Li</t>
+  </si>
+  <si>
+    <t>Elsa E. U. Poe</t>
+  </si>
+  <si>
+    <t>Flo F. V. Rye</t>
+  </si>
+  <si>
+    <t>Gus G. W. Smith</t>
+  </si>
+  <si>
+    <t>Hugo H. X. Watt</t>
+  </si>
+  <si>
+    <t>Ivy I. O. Cole</t>
+  </si>
+  <si>
+    <t>Jay J. P. Fox</t>
+  </si>
+  <si>
+    <t>Amy A. R. Jones</t>
+  </si>
+  <si>
+    <t>Beth B. S. King</t>
+  </si>
+  <si>
+    <t>Chad C. T. Li</t>
+  </si>
+  <si>
+    <t>Dan D. U. Poe</t>
+  </si>
+  <si>
+    <t>Elsa E. V. Rye</t>
   </si>
   <si>
     <t>Skills</t>
@@ -476,8 +548,8 @@
       <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
-        <v>21</v>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="E4" t="s">
         <v>21</v>
@@ -485,8 +557,8 @@
       <c r="F4" t="s">
         <v>21</v>
       </c>
-      <c r="G4" t="s">
-        <v>21</v>
+      <c r="G4" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="H4" t="s">
         <v>21</v>
@@ -494,26 +566,26 @@
       <c r="I4" t="s">
         <v>21</v>
       </c>
-      <c r="J4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O4" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" t="s">
-        <v>21</v>
+      <c r="J4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="Q4" t="s">
         <v>21</v>
@@ -521,8 +593,8 @@
       <c r="R4" t="s">
         <v>21</v>
       </c>
-      <c r="S4" t="s">
-        <v>21</v>
+      <c r="S4" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="T4" t="s">
         <v>21</v>
@@ -530,8 +602,8 @@
       <c r="U4" t="s">
         <v>21</v>
       </c>
-      <c r="V4" t="s">
-        <v>21</v>
+      <c r="V4" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5">
@@ -680,8 +752,8 @@
       <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" t="s">
-        <v>21</v>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="E7" t="s">
         <v>21</v>
@@ -689,8 +761,8 @@
       <c r="F7" t="s">
         <v>21</v>
       </c>
-      <c r="G7" t="s">
-        <v>21</v>
+      <c r="G7" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="H7" t="s">
         <v>21</v>
@@ -698,8 +770,8 @@
       <c r="I7" t="s">
         <v>21</v>
       </c>
-      <c r="J7" t="s">
-        <v>21</v>
+      <c r="J7" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="K7" t="s">
         <v>21</v>
@@ -707,8 +779,8 @@
       <c r="L7" t="s">
         <v>21</v>
       </c>
-      <c r="M7" t="s">
-        <v>21</v>
+      <c r="M7" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="N7" t="s">
         <v>21</v>
@@ -716,8 +788,8 @@
       <c r="O7" t="s">
         <v>21</v>
       </c>
-      <c r="P7" t="s">
-        <v>21</v>
+      <c r="P7" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="Q7" t="s">
         <v>21</v>
@@ -725,8 +797,8 @@
       <c r="R7" t="s">
         <v>21</v>
       </c>
-      <c r="S7" t="s">
-        <v>21</v>
+      <c r="S7" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="T7" t="s">
         <v>21</v>
@@ -734,8 +806,8 @@
       <c r="U7" t="s">
         <v>21</v>
       </c>
-      <c r="V7" t="s">
-        <v>21</v>
+      <c r="V7" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8">
@@ -748,8 +820,8 @@
       <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>22</v>
+      <c r="D8" t="s">
+        <v>21</v>
       </c>
       <c r="E8" t="s">
         <v>21</v>
@@ -757,8 +829,8 @@
       <c r="F8" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>22</v>
+      <c r="G8" t="s">
+        <v>21</v>
       </c>
       <c r="H8" t="s">
         <v>21</v>
@@ -766,8 +838,8 @@
       <c r="I8" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>22</v>
+      <c r="J8" t="s">
+        <v>21</v>
       </c>
       <c r="K8" t="s">
         <v>21</v>
@@ -775,8 +847,8 @@
       <c r="L8" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="2" t="s">
-        <v>22</v>
+      <c r="M8" t="s">
+        <v>21</v>
       </c>
       <c r="N8" t="s">
         <v>21</v>
@@ -784,8 +856,8 @@
       <c r="O8" t="s">
         <v>21</v>
       </c>
-      <c r="P8" s="2" t="s">
-        <v>22</v>
+      <c r="P8" t="s">
+        <v>21</v>
       </c>
       <c r="Q8" t="s">
         <v>21</v>
@@ -793,8 +865,8 @@
       <c r="R8" t="s">
         <v>21</v>
       </c>
-      <c r="S8" s="2" t="s">
-        <v>22</v>
+      <c r="S8" t="s">
+        <v>21</v>
       </c>
       <c r="T8" t="s">
         <v>21</v>
@@ -802,8 +874,8 @@
       <c r="U8" t="s">
         <v>21</v>
       </c>
-      <c r="V8" s="2" t="s">
-        <v>22</v>
+      <c r="V8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9">
@@ -884,8 +956,8 @@
       <c r="C10" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>22</v>
+      <c r="D10" t="s">
+        <v>21</v>
       </c>
       <c r="E10" t="s">
         <v>21</v>
@@ -893,8 +965,8 @@
       <c r="F10" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>22</v>
+      <c r="G10" t="s">
+        <v>21</v>
       </c>
       <c r="H10" t="s">
         <v>21</v>
@@ -902,26 +974,26 @@
       <c r="I10" t="s">
         <v>21</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>22</v>
+      <c r="J10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O10" t="s">
+        <v>21</v>
+      </c>
+      <c r="P10" t="s">
+        <v>21</v>
       </c>
       <c r="Q10" t="s">
         <v>21</v>
@@ -929,8 +1001,8 @@
       <c r="R10" t="s">
         <v>21</v>
       </c>
-      <c r="S10" s="2" t="s">
-        <v>22</v>
+      <c r="S10" t="s">
+        <v>21</v>
       </c>
       <c r="T10" t="s">
         <v>21</v>
@@ -938,8 +1010,8 @@
       <c r="U10" t="s">
         <v>21</v>
       </c>
-      <c r="V10" s="2" t="s">
-        <v>22</v>
+      <c r="V10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11">
@@ -952,8 +1024,8 @@
       <c r="C11" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>22</v>
+      <c r="D11" t="s">
+        <v>21</v>
       </c>
       <c r="E11" t="s">
         <v>21</v>
@@ -961,8 +1033,8 @@
       <c r="F11" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>22</v>
+      <c r="G11" t="s">
+        <v>21</v>
       </c>
       <c r="H11" t="s">
         <v>21</v>
@@ -970,26 +1042,26 @@
       <c r="I11" t="s">
         <v>21</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>22</v>
+      <c r="J11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" t="s">
+        <v>21</v>
+      </c>
+      <c r="P11" t="s">
+        <v>21</v>
       </c>
       <c r="Q11" t="s">
         <v>21</v>
@@ -997,8 +1069,8 @@
       <c r="R11" t="s">
         <v>21</v>
       </c>
-      <c r="S11" s="2" t="s">
-        <v>22</v>
+      <c r="S11" t="s">
+        <v>21</v>
       </c>
       <c r="T11" t="s">
         <v>21</v>
@@ -1006,8 +1078,8 @@
       <c r="U11" t="s">
         <v>21</v>
       </c>
-      <c r="V11" s="2" t="s">
-        <v>22</v>
+      <c r="V11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12">
@@ -1020,8 +1092,8 @@
       <c r="C12" t="s">
         <v>21</v>
       </c>
-      <c r="D12" t="s">
-        <v>21</v>
+      <c r="D12" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
@@ -1029,8 +1101,8 @@
       <c r="F12" t="s">
         <v>21</v>
       </c>
-      <c r="G12" t="s">
-        <v>21</v>
+      <c r="G12" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="H12" t="s">
         <v>21</v>
@@ -1038,8 +1110,8 @@
       <c r="I12" t="s">
         <v>21</v>
       </c>
-      <c r="J12" t="s">
-        <v>21</v>
+      <c r="J12" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="K12" t="s">
         <v>21</v>
@@ -1047,8 +1119,8 @@
       <c r="L12" t="s">
         <v>21</v>
       </c>
-      <c r="M12" t="s">
-        <v>21</v>
+      <c r="M12" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="N12" t="s">
         <v>21</v>
@@ -1056,8 +1128,8 @@
       <c r="O12" t="s">
         <v>21</v>
       </c>
-      <c r="P12" t="s">
-        <v>21</v>
+      <c r="P12" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="Q12" t="s">
         <v>21</v>
@@ -1065,8 +1137,8 @@
       <c r="R12" t="s">
         <v>21</v>
       </c>
-      <c r="S12" t="s">
-        <v>21</v>
+      <c r="S12" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="T12" t="s">
         <v>21</v>
@@ -1074,8 +1146,8 @@
       <c r="U12" t="s">
         <v>21</v>
       </c>
-      <c r="V12" t="s">
-        <v>21</v>
+      <c r="V12" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1939,6 +2011,1638 @@
         <v>22</v>
       </c>
       <c r="V13" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N14" t="s">
+        <v>22</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P14" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>22</v>
+      </c>
+      <c r="R14" t="s">
+        <v>22</v>
+      </c>
+      <c r="S14" t="s">
+        <v>22</v>
+      </c>
+      <c r="T14" t="s">
+        <v>22</v>
+      </c>
+      <c r="U14" t="s">
+        <v>22</v>
+      </c>
+      <c r="V14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" t="s">
+        <v>22</v>
+      </c>
+      <c r="L15" t="s">
+        <v>22</v>
+      </c>
+      <c r="M15" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" t="s">
+        <v>22</v>
+      </c>
+      <c r="O15" t="s">
+        <v>22</v>
+      </c>
+      <c r="P15" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>22</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="T15" t="s">
+        <v>22</v>
+      </c>
+      <c r="U15" t="s">
+        <v>22</v>
+      </c>
+      <c r="V15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" t="s">
+        <v>22</v>
+      </c>
+      <c r="O16" t="s">
+        <v>22</v>
+      </c>
+      <c r="P16" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>22</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="S16" t="s">
+        <v>22</v>
+      </c>
+      <c r="T16" t="s">
+        <v>22</v>
+      </c>
+      <c r="U16" t="s">
+        <v>22</v>
+      </c>
+      <c r="V16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" t="s">
+        <v>22</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P17" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>22</v>
+      </c>
+      <c r="R17" t="s">
+        <v>22</v>
+      </c>
+      <c r="S17" t="s">
+        <v>22</v>
+      </c>
+      <c r="T17" t="s">
+        <v>22</v>
+      </c>
+      <c r="U17" t="s">
+        <v>22</v>
+      </c>
+      <c r="V17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" t="s">
+        <v>22</v>
+      </c>
+      <c r="O18" t="s">
+        <v>22</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>22</v>
+      </c>
+      <c r="R18" t="s">
+        <v>22</v>
+      </c>
+      <c r="S18" t="s">
+        <v>22</v>
+      </c>
+      <c r="T18" t="s">
+        <v>22</v>
+      </c>
+      <c r="U18" t="s">
+        <v>22</v>
+      </c>
+      <c r="V18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N19" t="s">
+        <v>22</v>
+      </c>
+      <c r="O19" t="s">
+        <v>22</v>
+      </c>
+      <c r="P19" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>22</v>
+      </c>
+      <c r="R19" t="s">
+        <v>22</v>
+      </c>
+      <c r="S19" t="s">
+        <v>22</v>
+      </c>
+      <c r="T19" t="s">
+        <v>22</v>
+      </c>
+      <c r="U19" t="s">
+        <v>22</v>
+      </c>
+      <c r="V19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" t="s">
+        <v>22</v>
+      </c>
+      <c r="M20" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O20" t="s">
+        <v>22</v>
+      </c>
+      <c r="P20" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>22</v>
+      </c>
+      <c r="R20" t="s">
+        <v>22</v>
+      </c>
+      <c r="S20" t="s">
+        <v>22</v>
+      </c>
+      <c r="T20" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="U20" t="s">
+        <v>22</v>
+      </c>
+      <c r="V20" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" t="s">
+        <v>22</v>
+      </c>
+      <c r="M21" t="s">
+        <v>22</v>
+      </c>
+      <c r="N21" t="s">
+        <v>22</v>
+      </c>
+      <c r="O21" t="s">
+        <v>22</v>
+      </c>
+      <c r="P21" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="R21" t="s">
+        <v>22</v>
+      </c>
+      <c r="S21" t="s">
+        <v>22</v>
+      </c>
+      <c r="T21" t="s">
+        <v>22</v>
+      </c>
+      <c r="U21" t="s">
+        <v>22</v>
+      </c>
+      <c r="V21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" t="s">
+        <v>22</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P22" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>22</v>
+      </c>
+      <c r="R22" t="s">
+        <v>22</v>
+      </c>
+      <c r="S22" t="s">
+        <v>22</v>
+      </c>
+      <c r="T22" t="s">
+        <v>22</v>
+      </c>
+      <c r="U22" t="s">
+        <v>22</v>
+      </c>
+      <c r="V22" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" t="s">
+        <v>22</v>
+      </c>
+      <c r="K23" t="s">
+        <v>22</v>
+      </c>
+      <c r="L23" t="s">
+        <v>22</v>
+      </c>
+      <c r="M23" t="s">
+        <v>22</v>
+      </c>
+      <c r="N23" t="s">
+        <v>22</v>
+      </c>
+      <c r="O23" t="s">
+        <v>22</v>
+      </c>
+      <c r="P23" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>22</v>
+      </c>
+      <c r="R23" t="s">
+        <v>22</v>
+      </c>
+      <c r="S23" t="s">
+        <v>22</v>
+      </c>
+      <c r="T23" t="s">
+        <v>22</v>
+      </c>
+      <c r="U23" t="s">
+        <v>22</v>
+      </c>
+      <c r="V23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K24" t="s">
+        <v>22</v>
+      </c>
+      <c r="L24" t="s">
+        <v>22</v>
+      </c>
+      <c r="M24" t="s">
+        <v>22</v>
+      </c>
+      <c r="N24" t="s">
+        <v>22</v>
+      </c>
+      <c r="O24" t="s">
+        <v>22</v>
+      </c>
+      <c r="P24" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>22</v>
+      </c>
+      <c r="R24" t="s">
+        <v>22</v>
+      </c>
+      <c r="S24" t="s">
+        <v>22</v>
+      </c>
+      <c r="T24" t="s">
+        <v>22</v>
+      </c>
+      <c r="U24" t="s">
+        <v>22</v>
+      </c>
+      <c r="V24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" t="s">
+        <v>22</v>
+      </c>
+      <c r="K25" t="s">
+        <v>22</v>
+      </c>
+      <c r="L25" t="s">
+        <v>22</v>
+      </c>
+      <c r="M25" t="s">
+        <v>22</v>
+      </c>
+      <c r="N25" t="s">
+        <v>22</v>
+      </c>
+      <c r="O25" t="s">
+        <v>22</v>
+      </c>
+      <c r="P25" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>22</v>
+      </c>
+      <c r="R25" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="S25" t="s">
+        <v>22</v>
+      </c>
+      <c r="T25" t="s">
+        <v>22</v>
+      </c>
+      <c r="U25" t="s">
+        <v>22</v>
+      </c>
+      <c r="V25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" t="s">
+        <v>22</v>
+      </c>
+      <c r="K26" t="s">
+        <v>22</v>
+      </c>
+      <c r="L26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M26" t="s">
+        <v>22</v>
+      </c>
+      <c r="N26" t="s">
+        <v>22</v>
+      </c>
+      <c r="O26" t="s">
+        <v>22</v>
+      </c>
+      <c r="P26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>22</v>
+      </c>
+      <c r="R26" t="s">
+        <v>22</v>
+      </c>
+      <c r="S26" t="s">
+        <v>22</v>
+      </c>
+      <c r="T26" t="s">
+        <v>22</v>
+      </c>
+      <c r="U26" t="s">
+        <v>22</v>
+      </c>
+      <c r="V26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" t="s">
+        <v>22</v>
+      </c>
+      <c r="K27" t="s">
+        <v>22</v>
+      </c>
+      <c r="L27" t="s">
+        <v>22</v>
+      </c>
+      <c r="M27" t="s">
+        <v>22</v>
+      </c>
+      <c r="N27" t="s">
+        <v>22</v>
+      </c>
+      <c r="O27" t="s">
+        <v>22</v>
+      </c>
+      <c r="P27" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>22</v>
+      </c>
+      <c r="R27" t="s">
+        <v>22</v>
+      </c>
+      <c r="S27" t="s">
+        <v>22</v>
+      </c>
+      <c r="T27" t="s">
+        <v>22</v>
+      </c>
+      <c r="U27" t="s">
+        <v>22</v>
+      </c>
+      <c r="V27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" t="s">
+        <v>22</v>
+      </c>
+      <c r="K28" t="s">
+        <v>22</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M28" t="s">
+        <v>22</v>
+      </c>
+      <c r="N28" t="s">
+        <v>22</v>
+      </c>
+      <c r="O28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P28" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>22</v>
+      </c>
+      <c r="R28" t="s">
+        <v>22</v>
+      </c>
+      <c r="S28" t="s">
+        <v>22</v>
+      </c>
+      <c r="T28" t="s">
+        <v>22</v>
+      </c>
+      <c r="U28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="V28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" t="s">
+        <v>22</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J29" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" t="s">
+        <v>22</v>
+      </c>
+      <c r="L29" t="s">
+        <v>22</v>
+      </c>
+      <c r="M29" t="s">
+        <v>22</v>
+      </c>
+      <c r="N29" t="s">
+        <v>22</v>
+      </c>
+      <c r="O29" t="s">
+        <v>22</v>
+      </c>
+      <c r="P29" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>22</v>
+      </c>
+      <c r="R29" t="s">
+        <v>22</v>
+      </c>
+      <c r="S29" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="T29" t="s">
+        <v>22</v>
+      </c>
+      <c r="U29" t="s">
+        <v>22</v>
+      </c>
+      <c r="V29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" t="s">
+        <v>22</v>
+      </c>
+      <c r="J30" t="s">
+        <v>22</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L30" t="s">
+        <v>22</v>
+      </c>
+      <c r="M30" t="s">
+        <v>22</v>
+      </c>
+      <c r="N30" t="s">
+        <v>22</v>
+      </c>
+      <c r="O30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P30" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>22</v>
+      </c>
+      <c r="R30" t="s">
+        <v>22</v>
+      </c>
+      <c r="S30" t="s">
+        <v>22</v>
+      </c>
+      <c r="T30" t="s">
+        <v>22</v>
+      </c>
+      <c r="U30" t="s">
+        <v>22</v>
+      </c>
+      <c r="V30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H31" t="s">
+        <v>22</v>
+      </c>
+      <c r="I31" t="s">
+        <v>22</v>
+      </c>
+      <c r="J31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K31" t="s">
+        <v>22</v>
+      </c>
+      <c r="L31" t="s">
+        <v>22</v>
+      </c>
+      <c r="M31" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N31" t="s">
+        <v>22</v>
+      </c>
+      <c r="O31" t="s">
+        <v>22</v>
+      </c>
+      <c r="P31" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>22</v>
+      </c>
+      <c r="R31" t="s">
+        <v>22</v>
+      </c>
+      <c r="S31" t="s">
+        <v>22</v>
+      </c>
+      <c r="T31" t="s">
+        <v>22</v>
+      </c>
+      <c r="U31" t="s">
+        <v>22</v>
+      </c>
+      <c r="V31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" t="s">
+        <v>22</v>
+      </c>
+      <c r="F32" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H32" t="s">
+        <v>22</v>
+      </c>
+      <c r="I32" t="s">
+        <v>22</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K32" t="s">
+        <v>22</v>
+      </c>
+      <c r="L32" t="s">
+        <v>22</v>
+      </c>
+      <c r="M32" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N32" t="s">
+        <v>22</v>
+      </c>
+      <c r="O32" t="s">
+        <v>22</v>
+      </c>
+      <c r="P32" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>22</v>
+      </c>
+      <c r="R32" t="s">
+        <v>22</v>
+      </c>
+      <c r="S32" t="s">
+        <v>22</v>
+      </c>
+      <c r="T32" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="U32" t="s">
+        <v>22</v>
+      </c>
+      <c r="V32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" t="s">
+        <v>22</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" t="s">
+        <v>22</v>
+      </c>
+      <c r="I33" t="s">
+        <v>22</v>
+      </c>
+      <c r="J33" t="s">
+        <v>22</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L33" t="s">
+        <v>22</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N33" t="s">
+        <v>22</v>
+      </c>
+      <c r="O33" t="s">
+        <v>22</v>
+      </c>
+      <c r="P33" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>22</v>
+      </c>
+      <c r="R33" t="s">
+        <v>22</v>
+      </c>
+      <c r="S33" t="s">
+        <v>22</v>
+      </c>
+      <c r="T33" t="s">
+        <v>22</v>
+      </c>
+      <c r="U33" t="s">
+        <v>22</v>
+      </c>
+      <c r="V33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" t="s">
+        <v>22</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G34" t="s">
+        <v>22</v>
+      </c>
+      <c r="H34" t="s">
+        <v>22</v>
+      </c>
+      <c r="I34" t="s">
+        <v>22</v>
+      </c>
+      <c r="J34" t="s">
+        <v>22</v>
+      </c>
+      <c r="K34" t="s">
+        <v>22</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N34" t="s">
+        <v>22</v>
+      </c>
+      <c r="O34" t="s">
+        <v>22</v>
+      </c>
+      <c r="P34" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>22</v>
+      </c>
+      <c r="R34" t="s">
+        <v>22</v>
+      </c>
+      <c r="S34" t="s">
+        <v>22</v>
+      </c>
+      <c r="T34" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="U34" t="s">
+        <v>22</v>
+      </c>
+      <c r="V34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" t="s">
+        <v>22</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" t="s">
+        <v>22</v>
+      </c>
+      <c r="I35" t="s">
+        <v>22</v>
+      </c>
+      <c r="J35" t="s">
+        <v>22</v>
+      </c>
+      <c r="K35" t="s">
+        <v>22</v>
+      </c>
+      <c r="L35" t="s">
+        <v>22</v>
+      </c>
+      <c r="M35" t="s">
+        <v>22</v>
+      </c>
+      <c r="N35" t="s">
+        <v>22</v>
+      </c>
+      <c r="O35" t="s">
+        <v>22</v>
+      </c>
+      <c r="P35" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>22</v>
+      </c>
+      <c r="R35" t="s">
+        <v>22</v>
+      </c>
+      <c r="S35" t="s">
+        <v>22</v>
+      </c>
+      <c r="T35" t="s">
+        <v>22</v>
+      </c>
+      <c r="U35" t="s">
+        <v>22</v>
+      </c>
+      <c r="V35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36" t="s">
+        <v>22</v>
+      </c>
+      <c r="I36" t="s">
+        <v>22</v>
+      </c>
+      <c r="J36" t="s">
+        <v>22</v>
+      </c>
+      <c r="K36" t="s">
+        <v>22</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M36" t="s">
+        <v>22</v>
+      </c>
+      <c r="N36" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O36" t="s">
+        <v>22</v>
+      </c>
+      <c r="P36" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>22</v>
+      </c>
+      <c r="R36" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="S36" t="s">
+        <v>22</v>
+      </c>
+      <c r="T36" t="s">
+        <v>22</v>
+      </c>
+      <c r="U36" t="s">
+        <v>22</v>
+      </c>
+      <c r="V36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G37" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" t="s">
+        <v>22</v>
+      </c>
+      <c r="I37" t="s">
+        <v>22</v>
+      </c>
+      <c r="J37" t="s">
+        <v>22</v>
+      </c>
+      <c r="K37" t="s">
+        <v>22</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M37" t="s">
+        <v>22</v>
+      </c>
+      <c r="N37" t="s">
+        <v>22</v>
+      </c>
+      <c r="O37" t="s">
+        <v>22</v>
+      </c>
+      <c r="P37" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>22</v>
+      </c>
+      <c r="R37" t="s">
+        <v>22</v>
+      </c>
+      <c r="S37" t="s">
+        <v>22</v>
+      </c>
+      <c r="T37" t="s">
+        <v>22</v>
+      </c>
+      <c r="U37" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="V37" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1973,7 +3677,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s" s="1">
-        <v>34</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3">
@@ -1981,7 +3685,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4">
@@ -1989,7 +3693,7 @@
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -1997,7 +3701,7 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6">
@@ -2005,7 +3709,7 @@
         <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7">
@@ -2013,7 +3717,7 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8">
@@ -2021,7 +3725,7 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9">
@@ -2029,7 +3733,7 @@
         <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10">
@@ -2037,7 +3741,7 @@
         <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11">
@@ -2045,7 +3749,7 @@
         <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12">
@@ -2053,7 +3757,7 @@
         <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13">
@@ -2061,7 +3765,199 @@
         <v>33</v>
       </c>
       <c r="B13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
         <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2083,244 +3979,244 @@
     <row r="1"/>
     <row r="2">
       <c r="A2" t="s" s="1">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s" s="1">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s" s="1">
-        <v>41</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2345,7 +4241,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s" s="1">
-        <v>65</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3">
@@ -2353,7 +4249,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4">
@@ -2361,7 +4257,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -2369,7 +4265,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6">
@@ -2377,7 +4273,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7">
@@ -2385,7 +4281,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8">
@@ -2393,7 +4289,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9">
@@ -2401,7 +4297,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10">
@@ -2409,7 +4305,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11">
@@ -2417,7 +4313,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12">
@@ -2425,7 +4321,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2452,12 +4348,12 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>